<commit_message>
se sube la pleneacion del ciclo 3
</commit_message>
<xml_diff>
--- a/Projecto 3/Planeacion.xlsx
+++ b/Projecto 3/Planeacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="104">
   <si>
     <t>Orden de compra</t>
   </si>
@@ -316,6 +316,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Ciclo 1</t>
+  </si>
+  <si>
+    <t>Ciclo 2</t>
+  </si>
+  <si>
+    <t>Ciclo 3</t>
+  </si>
+  <si>
+    <t>ciclo 2</t>
   </si>
 </sst>
 </file>
@@ -387,7 +399,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,6 +427,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -515,6 +533,9 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,12 +850,12 @@
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -860,7 +881,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
@@ -900,8 +921,14 @@
         <f>SUM(H3:I3)</f>
         <v>33.127499999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -925,7 +952,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -948,7 +975,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -972,7 +999,7 @@
         <v>11.200000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1000,7 +1027,7 @@
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>1</v>
       </c>
@@ -1040,8 +1067,14 @@
         <f>SUM(H8:I8)</f>
         <v>57.203999999999994</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="M8" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1065,7 +1098,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -1089,7 +1122,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -1112,7 +1145,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -1136,7 +1169,7 @@
         <v>2.8000000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -1160,7 +1193,7 @@
         <v>12.600000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1184,7 +1217,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>2</v>
       </c>
@@ -1224,8 +1257,14 @@
         <f>SUM(H15:I15)</f>
         <v>102.24900000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="M15" s="27">
+        <v>0.34310000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
@@ -1248,8 +1287,14 @@
         <f>SUM(B16:E16)</f>
         <v>6.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L16" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="M16" s="27">
+        <v>0.65690000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -1273,7 +1318,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
@@ -1297,7 +1342,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -1321,7 +1366,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -1345,7 +1390,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
@@ -1369,7 +1414,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
@@ -1392,7 +1437,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -1416,7 +1461,7 @@
         <v>12.600000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
@@ -1440,7 +1485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
@@ -1464,7 +1509,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
@@ -1488,7 +1533,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>66</v>
       </c>
@@ -1512,7 +1557,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>3</v>
       </c>
@@ -1552,8 +1597,14 @@
         <f>SUM(H28:I28)</f>
         <v>132.67800000000003</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L28" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="M28" s="27">
+        <v>0.62560000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>68</v>
       </c>
@@ -1576,8 +1627,14 @@
         <f>SUM(B29:E29)</f>
         <v>6.2</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L29" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="M29" s="27">
+        <v>0.34439999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>69</v>
       </c>
@@ -1601,7 +1658,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>70</v>
       </c>
@@ -1625,7 +1682,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>71</v>
       </c>
@@ -1649,7 +1706,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>72</v>
       </c>
@@ -1673,7 +1730,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>73</v>
       </c>
@@ -1697,7 +1754,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>74</v>
       </c>
@@ -1721,7 +1778,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>75</v>
       </c>
@@ -1745,7 +1802,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>76</v>
       </c>
@@ -1768,7 +1825,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>77</v>
       </c>
@@ -1791,7 +1848,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>78</v>
       </c>
@@ -1815,7 +1872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>79</v>
       </c>
@@ -1839,7 +1896,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>80</v>
       </c>
@@ -1863,7 +1920,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>81</v>
       </c>
@@ -1887,7 +1944,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>82</v>
       </c>
@@ -1911,7 +1968,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>83</v>
       </c>
@@ -1935,7 +1992,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>4</v>
       </c>
@@ -1975,8 +2032,14 @@
         <f>SUM(H45:I45)</f>
         <v>81.522000000000006</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L45" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="M45" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>84</v>
       </c>
@@ -2000,7 +2063,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>85</v>
       </c>
@@ -2024,7 +2087,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>86</v>
       </c>
@@ -2570,12 +2633,135 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1">
+        <v>125</v>
+      </c>
+      <c r="E1">
+        <f>SUM(B2:B3)</f>
+        <v>90.331500000000005</v>
+      </c>
+      <c r="G1">
+        <v>35</v>
+      </c>
+      <c r="H1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="22">
+        <v>33.127499999999998</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="H2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3">
+        <v>57.204000000000001</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="G3">
+        <f>(G1*H2)/H1</f>
+        <v>34.313725490196077</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3">
+        <f>H3-G3</f>
+        <v>65.686274509803923</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>SUM(B1:B5)</f>
+        <v>490.33150000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f>F7-F8</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>B4-F9</f>
+        <v>83</v>
+      </c>
+      <c r="H10">
+        <v>132.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f>(F10*H11)/H10</f>
+        <v>62.556526982212837</v>
+      </c>
+      <c r="H12">
+        <f>H11-F12</f>
+        <v>37.443473017787163</v>
+      </c>
+      <c r="I12">
+        <v>81.52</v>
+      </c>
+      <c r="J12">
+        <f>I12+H12</f>
+        <v>118.96347301778715</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>